<commit_message>
Exploratory analaysis of fecal coliform exceeding 200 cfu/100ml
</commit_message>
<xml_diff>
--- a/Tables/table_1.xlsx
+++ b/Tables/table_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashaedmondson/Desktop/Environmental_Data_Analytics_2020/FinalProject/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E3F1FD-B57E-4147-8985-CD9050716840}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE23BEC-6B03-7C45-9E7A-2431D8B4D86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1020" windowWidth="25040" windowHeight="13740" xr2:uid="{517CDC89-D34B-D340-A9FB-C4BAE6F925E2}"/>
+    <workbookView xWindow="560" yWindow="1000" windowWidth="25040" windowHeight="13740" xr2:uid="{517CDC89-D34B-D340-A9FB-C4BAE6F925E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Parameter</t>
   </si>
@@ -54,12 +54,18 @@
   </si>
   <si>
     <t xml:space="preserve">Fecal Coliform 0.7 micron </t>
+  </si>
+  <si>
+    <t>Decmeber 31, 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,7 +98,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +416,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,8 +469,8 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>43465</v>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished formatting tables and inputting in codes for figures, running new stat analysis
</commit_message>
<xml_diff>
--- a/Tables/table_1.xlsx
+++ b/Tables/table_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashaedmondson/Desktop/Environmental_Data_Analytics_2020/FinalProject/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE23BEC-6B03-7C45-9E7A-2431D8B4D86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F37D5AD-BE6E-424E-A1A9-7C0D8C6959BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="1000" windowWidth="25040" windowHeight="13740" xr2:uid="{517CDC89-D34B-D340-A9FB-C4BAE6F925E2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Parameter</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Decmeber 31, 2018</t>
+  </si>
+  <si>
+    <t>Janurary 1, 1970</t>
   </si>
 </sst>
 </file>
@@ -64,12 +67,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,7 +107,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +425,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,8 +470,8 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>25569</v>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -474,6 +483,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>